<commit_message>
Included only people w/ all 4 outcomes (didn't lose any drug users)
</commit_message>
<xml_diff>
--- a/Project1/Reports/DemographicsTable09272017_formatted.xlsx
+++ b/Project1/Reports/DemographicsTable09272017_formatted.xlsx
@@ -33,25 +33,25 @@
     <t>Age at baseline</t>
   </si>
   <si>
-    <t>43.27 ± 8.78</t>
+    <t>43.26 ± 8.72</t>
   </si>
   <si>
     <t>44.62 ± 9.49</t>
   </si>
   <si>
-    <t>43.16 ± 8.72</t>
+    <t>43.14 ± 8.65</t>
   </si>
   <si>
     <t>BMI at baseline</t>
   </si>
   <si>
-    <t>25.26 ± 4.41</t>
+    <t>25.21 ± 4.34</t>
   </si>
   <si>
     <t>23.62 ± 3.45</t>
   </si>
   <si>
-    <t>25.39 ± 4.46</t>
+    <t>25.34 ± 4.39</t>
   </si>
   <si>
     <t>Alcohol use at baseline</t>
@@ -60,25 +60,25 @@
     <t>13 or fewer drinks per week</t>
   </si>
   <si>
-    <t>471 (93.08)</t>
+    <t>443 (93.07)</t>
   </si>
   <si>
     <t>37 (94.87)</t>
   </si>
   <si>
-    <t>434 (92.93)</t>
+    <t>406 (92.91)</t>
   </si>
   <si>
     <t>&gt; 13 drinks per week</t>
   </si>
   <si>
-    <t>35 (6.92)</t>
+    <t>33 (6.93)</t>
   </si>
   <si>
     <t>2 (5.13)</t>
   </si>
   <si>
-    <t>33 (7.07)</t>
+    <t>31 (7.09)</t>
   </si>
   <si>
     <t>Smoking status at baseline</t>
@@ -87,25 +87,25 @@
     <t>Never/former</t>
   </si>
   <si>
-    <t>310 (61.26)</t>
+    <t>291 (61.13)</t>
   </si>
   <si>
     <t>9 (23.08)</t>
   </si>
   <si>
-    <t>301 (64.45)</t>
+    <t>282 (64.53)</t>
   </si>
   <si>
     <t>Current</t>
   </si>
   <si>
-    <t>196 (38.74)</t>
+    <t>185 (38.87)</t>
   </si>
   <si>
     <t>30 (76.92)</t>
   </si>
   <si>
-    <t>166 (35.55)</t>
+    <t>155 (35.47)</t>
   </si>
   <si>
     <t>Income level at baseline</t>
@@ -114,34 +114,34 @@
     <t>&lt; $10,000</t>
   </si>
   <si>
-    <t>105 (20.75)</t>
+    <t>99 (20.8)</t>
   </si>
   <si>
     <t>14 (35.9)</t>
   </si>
   <si>
-    <t>91 (20.22)</t>
+    <t>85 (20.24)</t>
   </si>
   <si>
     <t>$10,000 - $40,000</t>
   </si>
   <si>
-    <t>210 (41.5)</t>
+    <t>196 (41.18)</t>
   </si>
   <si>
     <t>16 (41.03)</t>
   </si>
   <si>
-    <t>194 (43.11)</t>
+    <t>180 (42.86)</t>
   </si>
   <si>
     <t>&gt; $40,000</t>
   </si>
   <si>
-    <t>174 (34.39)</t>
-  </si>
-  <si>
-    <t>165 (36.67)</t>
+    <t>164 (34.45)</t>
+  </si>
+  <si>
+    <t>155 (36.9)</t>
   </si>
   <si>
     <t>Education at baseline</t>
@@ -150,22 +150,22 @@
     <t>HS or less</t>
   </si>
   <si>
-    <t>111 (21.94)</t>
-  </si>
-  <si>
-    <t>95 (20.34)</t>
+    <t>101 (21.22)</t>
+  </si>
+  <si>
+    <t>85 (19.45)</t>
   </si>
   <si>
     <t>&gt;HS</t>
   </si>
   <si>
-    <t>395 (78.06)</t>
+    <t>375 (78.78)</t>
   </si>
   <si>
     <t>23 (58.97)</t>
   </si>
   <si>
-    <t>372 (79.66)</t>
+    <t>352 (80.55)</t>
   </si>
   <si>
     <t>Adherence at 2 years</t>
@@ -174,25 +174,25 @@
     <t>&lt;95%</t>
   </si>
   <si>
-    <t>52 (10.28)</t>
+    <t>50 (10.5)</t>
   </si>
   <si>
     <t>1 (2.56)</t>
   </si>
   <si>
-    <t>51 (10.92)</t>
+    <t>49 (11.21)</t>
   </si>
   <si>
     <t>&gt;95%</t>
   </si>
   <si>
-    <t>454 (89.72)</t>
+    <t>426 (89.5)</t>
   </si>
   <si>
     <t>38 (97.44)</t>
   </si>
   <si>
-    <t>416 (89.08)</t>
+    <t>388 (88.79)</t>
   </si>
   <si>
     <t>Baseline log10 viral load</t>
@@ -210,37 +210,37 @@
     <t>Baseline CD4+ count</t>
   </si>
   <si>
-    <t>374.7 ± 199.7</t>
+    <t>373.53 ± 200.46</t>
   </si>
   <si>
     <t>352.18 ± 194.67</t>
   </si>
   <si>
-    <t>376.66 ± 200.22</t>
+    <t>375.44 ± 201.07</t>
   </si>
   <si>
     <t>Baseline SF36 MCS score</t>
   </si>
   <si>
-    <t>45.23 ± 13.49</t>
+    <t>44.89 ± 13.5</t>
   </si>
   <si>
     <t>42.31 ± 11.22</t>
   </si>
   <si>
-    <t>45.48 ± 13.65</t>
+    <t>45.12 ± 13.68</t>
   </si>
   <si>
     <t>Baseline SF36 PCS score</t>
   </si>
   <si>
-    <t>51.03 ± 9.11</t>
+    <t>51.04 ± 9.05</t>
   </si>
   <si>
     <t>47.7 ± 8.5</t>
   </si>
   <si>
-    <t>51.31 ± 9.11</t>
+    <t>51.34 ± 9.05</t>
   </si>
 </sst>
 </file>
@@ -796,9 +796,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -816,18 +815,7 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,7 +824,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1161,308 +1159,303 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    </row>
+    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    </row>
+    <row r="18" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>